<commit_message>
Included Laboratory Results Units
</commit_message>
<xml_diff>
--- a/ListOfVariables.xlsx
+++ b/ListOfVariables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcarrasco\Documents\PFIS_PhD\Codigo\Models\CodeToPublish\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcarrasco\Documents\PFIS_PhD\Article_AllModels\Documentacion\CodeToPublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC1AD05-4C09-4950-85A8-D52AC280316A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA7FCE2-E599-4E13-8DAF-B6988DDCA7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -355,117 +355,78 @@
     <t>Number of Creatinine measurements</t>
   </si>
   <si>
-    <t>Mean value of Creatinine measurements</t>
-  </si>
-  <si>
     <t>Number of Creatinine measurements out of range</t>
   </si>
   <si>
     <t>Number of Albumine measurements</t>
   </si>
   <si>
-    <t>Mean value of Albumine measurements</t>
-  </si>
-  <si>
     <t>Number of Albumine measurements out of range</t>
   </si>
   <si>
     <t>Number of HDL measurements</t>
   </si>
   <si>
-    <t>Mean value of HDL measurements</t>
-  </si>
-  <si>
     <t>Number of HDL measurements out of range</t>
   </si>
   <si>
     <t>Number of LDL measurements</t>
   </si>
   <si>
-    <t>Mean value of LDL measurements</t>
-  </si>
-  <si>
     <t>Number of LDL measurements out of range</t>
   </si>
   <si>
     <t>Number of Total Cholesterol measurements</t>
   </si>
   <si>
-    <t>Mean value of Total Cholesterol measurements</t>
-  </si>
-  <si>
     <t>Number of Total Cholesterol measurements out of range</t>
   </si>
   <si>
     <t>Number of GGT measurements</t>
   </si>
   <si>
-    <t>Mean value of GGT measurements</t>
-  </si>
-  <si>
     <t>Number of GGT measurements out of range</t>
   </si>
   <si>
     <t>Number of GOT measurements</t>
   </si>
   <si>
-    <t>Mean value of GOT measurements</t>
-  </si>
-  <si>
     <t>Number of GOT measurements out of range</t>
   </si>
   <si>
     <t>Number of GPT measurements</t>
   </si>
   <si>
-    <t>Mean value of GPT measurements</t>
-  </si>
-  <si>
     <t>Number of GPT measurements out of range</t>
   </si>
   <si>
     <t>Number of Leukocytes measurements</t>
   </si>
   <si>
-    <t>Mean value of Leukocytes measurements</t>
-  </si>
-  <si>
     <t>Number of Leukocytes measurements out of range</t>
   </si>
   <si>
     <t>Number of Neutrophiles (Total) measurements</t>
   </si>
   <si>
-    <t>Mean value of Neutrophiles (Total) measurements</t>
-  </si>
-  <si>
     <t>Number of Neutrophiles (Total) measurements out of range</t>
   </si>
   <si>
     <t>Number of Glucose measurements</t>
   </si>
   <si>
-    <t>Mean value of Glucose measurements</t>
-  </si>
-  <si>
     <t>Number of Glucose measurements out of range</t>
   </si>
   <si>
     <t>Number of HbA1c measurements</t>
   </si>
   <si>
-    <t>Mean value of HbA1c measurements</t>
-  </si>
-  <si>
     <t>Number of HbA1c measurements out of range</t>
   </si>
   <si>
     <t>Number of Platelets measurements</t>
   </si>
   <si>
-    <t>Mean value of Platelets measurements</t>
-  </si>
-  <si>
     <t>Number of Platelets measurements out of range</t>
   </si>
   <si>
@@ -940,27 +901,12 @@
     <t>Number of alkaline phosphatase measurements</t>
   </si>
   <si>
-    <t>Mean value of alkaline phosphatase measurements</t>
-  </si>
-  <si>
     <t>Number of alkaline phosphatase measurements out of range</t>
   </si>
   <si>
-    <t>Number of Alpha-1-Antitipsine measurements</t>
-  </si>
-  <si>
-    <t>Mean value of Alpha-1-Antitipsine measurements</t>
-  </si>
-  <si>
-    <t>Number of Alpha-1-Antitipsine measurements out of range</t>
-  </si>
-  <si>
     <t>Number of Glomerular Filtration (CKD-EPI) measurements</t>
   </si>
   <si>
-    <t>Mean value of Glomerular Filtration (CKD-EPI) measurements</t>
-  </si>
-  <si>
     <t>Number of Glomerular Filtration (CKD-EPI) measurements out of range</t>
   </si>
   <si>
@@ -1006,18 +952,12 @@
     <t>Number of hemoglobin (HCM) measurements</t>
   </si>
   <si>
-    <t>Mean value of hemoglobin (HCM) measurements</t>
-  </si>
-  <si>
     <t>Number of hemoglobin (HCM) measurements out of range</t>
   </si>
   <si>
     <t>Number of erythrocytes measurements</t>
   </si>
   <si>
-    <t>Mean value of erythrocytes measurements</t>
-  </si>
-  <si>
     <t>Number of erythrocytes measurements out of range</t>
   </si>
   <si>
@@ -1039,9 +979,6 @@
     <t>Number of hemoglobin measurements</t>
   </si>
   <si>
-    <t>Mean value of hemoglobin measurements</t>
-  </si>
-  <si>
     <t>Number of hemoglobin measurements out of range</t>
   </si>
   <si>
@@ -1069,9 +1006,6 @@
     <t>Number of Glomerular Filtration (MDRD) measurements</t>
   </si>
   <si>
-    <t>Mean value of  Glomerular Filtration (MDRD) measurements</t>
-  </si>
-  <si>
     <t>Number of  Glomerular Filtration (MDRD) measurements out of range</t>
   </si>
   <si>
@@ -1108,9 +1042,6 @@
     <t>Number of triglycerides measurements</t>
   </si>
   <si>
-    <t>Mean value of triglycerides measurements</t>
-  </si>
-  <si>
     <t>Number of triglycerides measurements out of range</t>
   </si>
   <si>
@@ -1556,6 +1487,75 @@
   </si>
   <si>
     <t>Y_VenousLymphatic</t>
+  </si>
+  <si>
+    <t>Mean value of HDL measurements (mg/dL)</t>
+  </si>
+  <si>
+    <t>Mean value of Total Cholesterol measurements (mg/dL)</t>
+  </si>
+  <si>
+    <t>Mean value of LDL measurements (mg/dL)</t>
+  </si>
+  <si>
+    <t>Mean value of hemoglobin (HCM) measurements (pg)</t>
+  </si>
+  <si>
+    <t>Mean value of GPT measurements (U/L)</t>
+  </si>
+  <si>
+    <t>Mean value of GOT measurements (U/L)</t>
+  </si>
+  <si>
+    <t>Mean value of GGT measurements (U/L)</t>
+  </si>
+  <si>
+    <t>Mean value of triglycerides measurements (mg/dL)</t>
+  </si>
+  <si>
+    <t>Mean value of erythrocytes measurements (K/mcL)</t>
+  </si>
+  <si>
+    <t>Mean value of Leukocytes measurements  (K/mcL)</t>
+  </si>
+  <si>
+    <t>Mean value of Neutrophiles (Total) measurements  (10^3 K/mcL)</t>
+  </si>
+  <si>
+    <t>Mean value of Platelets measurements  (K/mcL)</t>
+  </si>
+  <si>
+    <t>Mean value of hemoglobin measurements (g/dL)</t>
+  </si>
+  <si>
+    <t>Mean value of  Glomerular Filtration (MDRD) measurements (ml/min/1.73m2)</t>
+  </si>
+  <si>
+    <t>Mean value of Glomerular Filtration (CKD-EPI) measurements (ml/min/1.73m2)</t>
+  </si>
+  <si>
+    <t>Mean value of HbA1c measurements (mmol/mol)</t>
+  </si>
+  <si>
+    <t>Mean value of Glucose measurements (mg/dL)</t>
+  </si>
+  <si>
+    <t>Mean value of alkaline phosphatase measurements (U/L)</t>
+  </si>
+  <si>
+    <t>Mean value of Creatinine measurements (mg/dL)</t>
+  </si>
+  <si>
+    <t>Mean value of Albumine measurements (g/dL)</t>
+  </si>
+  <si>
+    <t>Number of Alpha-1-Antitripsine measurements</t>
+  </si>
+  <si>
+    <t>Number of Alpha-1-Antitripsine measurements out of range</t>
+  </si>
+  <si>
+    <t>Mean value of Alpha-1-Antitripsine measurements (mg/dL)</t>
   </si>
 </sst>
 </file>
@@ -1571,18 +1571,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1597,14 +1591,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3155,7 +3147,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9277B9F4-5334-4D79-9E57-BB1838F53F2A}" name="TablaDinámica1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Domain">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9277B9F4-5334-4D79-9E57-BB1838F53F2A}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Domain">
   <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -3548,86 +3540,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D249"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B249" sqref="B2:B249"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="C3" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="C4" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" t="s">
         <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3635,13 +3627,13 @@
         <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
         <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3649,13 +3641,13 @@
         <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s">
         <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3663,13 +3655,13 @@
         <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
         <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3677,13 +3669,13 @@
         <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3691,13 +3683,13 @@
         <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3705,13 +3697,13 @@
         <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="D11" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3719,13 +3711,13 @@
         <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3733,13 +3725,13 @@
         <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3747,13 +3739,13 @@
         <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3761,13 +3753,13 @@
         <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C15" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="D15" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3775,13 +3767,13 @@
         <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C16" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3789,13 +3781,13 @@
         <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="C17" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3803,13 +3795,13 @@
         <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C18" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="D18" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3817,13 +3809,13 @@
         <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C19" t="s">
         <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3831,13 +3823,13 @@
         <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C20" t="s">
         <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3845,13 +3837,13 @@
         <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s">
         <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3859,13 +3851,13 @@
         <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="C22" t="s">
         <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3873,13 +3865,13 @@
         <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C23" t="s">
         <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3887,13 +3879,13 @@
         <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="D24" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3901,13 +3893,13 @@
         <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C25" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3915,13 +3907,13 @@
         <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C26" t="s">
         <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,13 +3921,13 @@
         <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="C27" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="D27" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3943,13 +3935,13 @@
         <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="D28" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3957,13 +3949,13 @@
         <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="C29" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="D29" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,13 +3963,13 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C30" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="D30" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3985,13 +3977,13 @@
         <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C31" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D31" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3999,13 +3991,13 @@
         <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C32" t="s">
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4013,13 +4005,13 @@
         <v>85</v>
       </c>
       <c r="B33" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C33" t="s">
         <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4027,13 +4019,13 @@
         <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="C34" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="D34" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4041,13 +4033,13 @@
         <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="D35" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4055,13 +4047,13 @@
         <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="D36" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4069,13 +4061,13 @@
         <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C37" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D37" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4083,13 +4075,13 @@
         <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C38" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="D38" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4097,13 +4089,13 @@
         <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="C39" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="D39" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4111,13 +4103,13 @@
         <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C40" t="s">
         <v>95</v>
       </c>
       <c r="D40" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4125,13 +4117,13 @@
         <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C41" t="s">
         <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4139,13 +4131,13 @@
         <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="C42" t="s">
         <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4153,13 +4145,13 @@
         <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="C43" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="D43" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4167,13 +4159,13 @@
         <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C44" t="s">
         <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,13 +4173,13 @@
         <v>85</v>
       </c>
       <c r="B45" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C45" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="D45" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4195,13 +4187,13 @@
         <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C46" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D46" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4209,13 +4201,13 @@
         <v>85</v>
       </c>
       <c r="B47" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C47" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="D47" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4223,13 +4215,13 @@
         <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="C48" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="D48" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4237,13 +4229,13 @@
         <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C49" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="D49" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,13 +4243,13 @@
         <v>85</v>
       </c>
       <c r="B50" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C50" t="s">
         <v>99</v>
       </c>
       <c r="D50" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4265,13 +4257,13 @@
         <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="C51" t="s">
         <v>100</v>
       </c>
       <c r="D51" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4279,13 +4271,13 @@
         <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C52" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="D52" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4293,13 +4285,13 @@
         <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="C53" t="s">
         <v>101</v>
       </c>
       <c r="D53" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4307,13 +4299,13 @@
         <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C54" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D54" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4321,13 +4313,13 @@
         <v>85</v>
       </c>
       <c r="B55" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C55" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D55" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4335,13 +4327,13 @@
         <v>85</v>
       </c>
       <c r="B56" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C56" t="s">
         <v>102</v>
       </c>
       <c r="D56" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4349,13 +4341,13 @@
         <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C57" t="s">
         <v>103</v>
       </c>
       <c r="D57" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4363,13 +4355,13 @@
         <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="C58" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="D58" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4377,13 +4369,13 @@
         <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C59" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="D59" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4391,13 +4383,13 @@
         <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="C60" t="s">
         <v>104</v>
       </c>
       <c r="D60" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4405,13 +4397,13 @@
         <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="C61" t="s">
         <v>105</v>
       </c>
       <c r="D61" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4419,13 +4411,13 @@
         <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="C62" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="D62" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4433,13 +4425,13 @@
         <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="C63" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D63" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4447,13 +4439,13 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,13 +4453,13 @@
         <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4475,13 +4467,13 @@
         <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
       <c r="C66" t="s">
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4489,13 +4481,13 @@
         <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4503,13 +4495,13 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>408</v>
+        <v>385</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4517,13 +4509,13 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -4531,13 +4523,13 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="C70" t="s">
         <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4545,13 +4537,13 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
       <c r="C71" t="s">
         <v>11</v>
       </c>
       <c r="D71" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4559,13 +4551,13 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="C72" t="s">
         <v>12</v>
       </c>
       <c r="D72" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4573,13 +4565,13 @@
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
       <c r="C73" t="s">
         <v>13</v>
       </c>
       <c r="D73" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4587,13 +4579,13 @@
         <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>415</v>
+        <v>392</v>
       </c>
       <c r="C74" t="s">
         <v>14</v>
       </c>
       <c r="D74" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4601,13 +4593,13 @@
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
       <c r="C75" t="s">
         <v>15</v>
       </c>
       <c r="D75" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4615,13 +4607,13 @@
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>417</v>
+        <v>394</v>
       </c>
       <c r="C76" t="s">
         <v>16</v>
       </c>
       <c r="D76" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4629,13 +4621,13 @@
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
       <c r="C77" t="s">
         <v>17</v>
       </c>
       <c r="D77" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4643,13 +4635,13 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="C78" t="s">
         <v>18</v>
       </c>
       <c r="D78" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4657,13 +4649,13 @@
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
       <c r="C79" t="s">
         <v>19</v>
       </c>
       <c r="D79" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,13 +4663,13 @@
         <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
       <c r="C80" t="s">
         <v>20</v>
       </c>
       <c r="D80" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4685,13 +4677,13 @@
         <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
       <c r="C81" t="s">
         <v>21</v>
       </c>
       <c r="D81" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4699,13 +4691,13 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>412</v>
+        <v>389</v>
       </c>
       <c r="C82" t="s">
         <v>22</v>
       </c>
       <c r="D82" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4713,13 +4705,13 @@
         <v>7</v>
       </c>
       <c r="B83" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="C83" t="s">
         <v>23</v>
       </c>
       <c r="D83" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,13 +4719,13 @@
         <v>7</v>
       </c>
       <c r="B84" t="s">
-        <v>424</v>
+        <v>401</v>
       </c>
       <c r="C84" t="s">
         <v>24</v>
       </c>
       <c r="D84" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4741,13 +4733,13 @@
         <v>7</v>
       </c>
       <c r="B85" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
       <c r="C85" t="s">
         <v>25</v>
       </c>
       <c r="D85" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4755,13 +4747,13 @@
         <v>7</v>
       </c>
       <c r="B86" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="C86" t="s">
         <v>26</v>
       </c>
       <c r="D86" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4769,13 +4761,13 @@
         <v>7</v>
       </c>
       <c r="B87" t="s">
-        <v>427</v>
+        <v>404</v>
       </c>
       <c r="C87" t="s">
         <v>27</v>
       </c>
       <c r="D87" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4783,13 +4775,13 @@
         <v>7</v>
       </c>
       <c r="B88" t="s">
-        <v>428</v>
+        <v>405</v>
       </c>
       <c r="C88" t="s">
         <v>28</v>
       </c>
       <c r="D88" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4797,13 +4789,13 @@
         <v>7</v>
       </c>
       <c r="B89" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="C89" t="s">
         <v>29</v>
       </c>
       <c r="D89" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4811,13 +4803,13 @@
         <v>7</v>
       </c>
       <c r="B90" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="C90" t="s">
         <v>63</v>
       </c>
       <c r="D90" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4825,13 +4817,13 @@
         <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="C91" t="s">
         <v>30</v>
       </c>
       <c r="D91" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4839,13 +4831,13 @@
         <v>7</v>
       </c>
       <c r="B92" t="s">
-        <v>472</v>
+        <v>449</v>
       </c>
       <c r="C92" t="s">
         <v>31</v>
       </c>
       <c r="D92" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4853,13 +4845,13 @@
         <v>7</v>
       </c>
       <c r="B93" t="s">
-        <v>473</v>
+        <v>450</v>
       </c>
       <c r="C93" t="s">
         <v>32</v>
       </c>
       <c r="D93" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4867,13 +4859,13 @@
         <v>7</v>
       </c>
       <c r="B94" t="s">
-        <v>474</v>
+        <v>451</v>
       </c>
       <c r="C94" t="s">
         <v>33</v>
       </c>
       <c r="D94" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,13 +4873,13 @@
         <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
       <c r="C95" t="s">
         <v>34</v>
       </c>
       <c r="D95" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4895,13 +4887,13 @@
         <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="C96" t="s">
         <v>35</v>
       </c>
       <c r="D96" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4909,13 +4901,13 @@
         <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="C97" t="s">
         <v>36</v>
       </c>
       <c r="D97" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4923,13 +4915,13 @@
         <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>481</v>
+        <v>458</v>
       </c>
       <c r="C98" t="s">
         <v>37</v>
       </c>
       <c r="D98" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4937,13 +4929,13 @@
         <v>7</v>
       </c>
       <c r="B99" t="s">
-        <v>485</v>
+        <v>462</v>
       </c>
       <c r="C99" t="s">
         <v>38</v>
       </c>
       <c r="D99" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4951,13 +4943,13 @@
         <v>7</v>
       </c>
       <c r="B100" t="s">
-        <v>482</v>
+        <v>459</v>
       </c>
       <c r="C100" t="s">
-        <v>483</v>
+        <v>460</v>
       </c>
       <c r="D100" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4965,13 +4957,13 @@
         <v>7</v>
       </c>
       <c r="B101" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
       <c r="C101" t="s">
         <v>39</v>
       </c>
       <c r="D101" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,13 +4971,13 @@
         <v>7</v>
       </c>
       <c r="B102" t="s">
-        <v>487</v>
+        <v>464</v>
       </c>
       <c r="C102" t="s">
         <v>40</v>
       </c>
       <c r="D102" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4993,13 +4985,13 @@
         <v>7</v>
       </c>
       <c r="B103" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C103" t="s">
         <v>64</v>
       </c>
       <c r="D103" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -5007,13 +4999,13 @@
         <v>7</v>
       </c>
       <c r="B104" t="s">
-        <v>486</v>
+        <v>463</v>
       </c>
       <c r="C104" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
       <c r="D104" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -5021,13 +5013,13 @@
         <v>7</v>
       </c>
       <c r="B105" t="s">
-        <v>478</v>
+        <v>455</v>
       </c>
       <c r="C105" t="s">
         <v>41</v>
       </c>
       <c r="D105" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -5035,13 +5027,13 @@
         <v>7</v>
       </c>
       <c r="B106" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
       <c r="C106" t="s">
         <v>42</v>
       </c>
       <c r="D106" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -5049,13 +5041,13 @@
         <v>7</v>
       </c>
       <c r="B107" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
       <c r="C107" t="s">
         <v>43</v>
       </c>
       <c r="D107" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -5063,13 +5055,13 @@
         <v>7</v>
       </c>
       <c r="B108" t="s">
-        <v>490</v>
+        <v>467</v>
       </c>
       <c r="C108" t="s">
         <v>44</v>
       </c>
       <c r="D108" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5077,13 +5069,13 @@
         <v>7</v>
       </c>
       <c r="B109" t="s">
-        <v>491</v>
+        <v>468</v>
       </c>
       <c r="C109" t="s">
         <v>45</v>
       </c>
       <c r="D109" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,13 +5083,13 @@
         <v>7</v>
       </c>
       <c r="B110" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
       <c r="C110" t="s">
         <v>46</v>
       </c>
       <c r="D110" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -5105,13 +5097,13 @@
         <v>7</v>
       </c>
       <c r="B111" t="s">
-        <v>493</v>
+        <v>470</v>
       </c>
       <c r="C111" t="s">
         <v>47</v>
       </c>
       <c r="D111" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -5119,13 +5111,13 @@
         <v>7</v>
       </c>
       <c r="B112" t="s">
-        <v>495</v>
+        <v>472</v>
       </c>
       <c r="C112" t="s">
         <v>48</v>
       </c>
       <c r="D112" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -5133,13 +5125,13 @@
         <v>7</v>
       </c>
       <c r="B113" t="s">
-        <v>494</v>
+        <v>471</v>
       </c>
       <c r="C113" t="s">
         <v>49</v>
       </c>
       <c r="D113" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -5147,13 +5139,13 @@
         <v>7</v>
       </c>
       <c r="B114" t="s">
-        <v>496</v>
+        <v>473</v>
       </c>
       <c r="C114" t="s">
         <v>50</v>
       </c>
       <c r="D114" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -5161,13 +5153,13 @@
         <v>7</v>
       </c>
       <c r="B115" t="s">
-        <v>497</v>
+        <v>474</v>
       </c>
       <c r="C115" t="s">
         <v>51</v>
       </c>
       <c r="D115" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -5175,13 +5167,13 @@
         <v>7</v>
       </c>
       <c r="B116" t="s">
-        <v>498</v>
+        <v>475</v>
       </c>
       <c r="C116" t="s">
         <v>52</v>
       </c>
       <c r="D116" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -5189,13 +5181,13 @@
         <v>7</v>
       </c>
       <c r="B117" t="s">
-        <v>499</v>
+        <v>476</v>
       </c>
       <c r="C117" t="s">
         <v>53</v>
       </c>
       <c r="D117" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5203,13 +5195,13 @@
         <v>7</v>
       </c>
       <c r="B118" t="s">
-        <v>500</v>
+        <v>477</v>
       </c>
       <c r="C118" t="s">
         <v>54</v>
       </c>
       <c r="D118" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5217,13 +5209,13 @@
         <v>7</v>
       </c>
       <c r="B119" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="C119" t="s">
         <v>55</v>
       </c>
       <c r="D119" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5231,13 +5223,13 @@
         <v>7</v>
       </c>
       <c r="B120" t="s">
-        <v>502</v>
+        <v>479</v>
       </c>
       <c r="C120" t="s">
         <v>56</v>
       </c>
       <c r="D120" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5245,13 +5237,13 @@
         <v>7</v>
       </c>
       <c r="B121" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
       <c r="C121" t="s">
         <v>57</v>
       </c>
       <c r="D121" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -5259,13 +5251,13 @@
         <v>7</v>
       </c>
       <c r="B122" t="s">
-        <v>504</v>
+        <v>481</v>
       </c>
       <c r="C122" t="s">
         <v>58</v>
       </c>
       <c r="D122" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -5273,13 +5265,13 @@
         <v>7</v>
       </c>
       <c r="B123" t="s">
-        <v>505</v>
+        <v>482</v>
       </c>
       <c r="C123" t="s">
         <v>59</v>
       </c>
       <c r="D123" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -5287,13 +5279,13 @@
         <v>7</v>
       </c>
       <c r="B124" t="s">
-        <v>506</v>
+        <v>483</v>
       </c>
       <c r="C124" t="s">
         <v>60</v>
       </c>
       <c r="D124" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -5301,13 +5293,13 @@
         <v>7</v>
       </c>
       <c r="B125" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
       <c r="C125" t="s">
         <v>61</v>
       </c>
       <c r="D125" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5315,13 +5307,13 @@
         <v>7</v>
       </c>
       <c r="B126" t="s">
-        <v>508</v>
+        <v>485</v>
       </c>
       <c r="C126" t="s">
         <v>62</v>
       </c>
       <c r="D126" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -5329,13 +5321,13 @@
         <v>7</v>
       </c>
       <c r="B127" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="C127" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
       <c r="D127" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5343,13 +5335,13 @@
         <v>68</v>
       </c>
       <c r="B128" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="C128" t="s">
         <v>65</v>
       </c>
       <c r="D128" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5357,13 +5349,13 @@
         <v>68</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D129" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -5371,531 +5363,531 @@
         <v>68</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D130" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="C131" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="D131" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B132" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="C132" t="s">
         <v>8</v>
       </c>
       <c r="D132" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B133" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="C133" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="D133" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B134" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
       <c r="C134" t="s">
         <v>5</v>
       </c>
       <c r="D134" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="C135" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="D135" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B136" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
       <c r="C136" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="D136" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="C137" t="s">
         <v>17</v>
       </c>
       <c r="D137" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="C138" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D138" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="C139" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="D139" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>137</v>
+      </c>
+      <c r="B140" t="s">
+        <v>417</v>
+      </c>
+      <c r="C140" t="s">
         <v>150</v>
       </c>
-      <c r="B140" t="s">
-        <v>440</v>
-      </c>
-      <c r="C140" t="s">
-        <v>163</v>
-      </c>
       <c r="D140" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B141" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
       <c r="C141" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="D141" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B142" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="C142" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="D142" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B143" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
       <c r="C143" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="D143" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B144" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="C144" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D144" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B145" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="C145" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D145" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B146" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="C146" t="s">
         <v>34</v>
       </c>
       <c r="D146" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B147" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="C147" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="D147" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B148" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
       <c r="C148" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="D148" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B149" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="C149" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D149" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B150" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
       <c r="C150" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D150" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B151" t="s">
-        <v>455</v>
+        <v>432</v>
       </c>
       <c r="C151" t="s">
         <v>43</v>
       </c>
       <c r="D151" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B152" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
       <c r="C152" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="D152" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B153" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
       <c r="C153" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="D153" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B154" t="s">
-        <v>465</v>
+        <v>442</v>
       </c>
       <c r="C154" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="D154" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B155" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="C155" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="D155" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B156" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
       <c r="C156" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D156" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B157" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
       <c r="C157" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D157" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B158" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="C158" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="D158" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B159" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="C159" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D159" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B160" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
       <c r="C160" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D160" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B161" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="C161" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="D161" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B162" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="C162" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="D162" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B163" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="C163" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D163" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B164" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="C164" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D164" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B165" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="C165" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="D165" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B166" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
       <c r="C166" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D166" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B167" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="C167" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="D167" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -5903,13 +5895,13 @@
         <v>106</v>
       </c>
       <c r="B168" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="C168" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D168" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -5917,13 +5909,13 @@
         <v>106</v>
       </c>
       <c r="B169" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="C169" t="s">
-        <v>305</v>
+        <v>506</v>
       </c>
       <c r="D169" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -5931,13 +5923,13 @@
         <v>106</v>
       </c>
       <c r="B170" t="s">
-        <v>361</v>
+        <v>338</v>
       </c>
       <c r="C170" t="s">
-        <v>306</v>
+        <v>508</v>
       </c>
       <c r="D170" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -5945,13 +5937,13 @@
         <v>106</v>
       </c>
       <c r="B171" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="C171" t="s">
-        <v>307</v>
+        <v>507</v>
       </c>
       <c r="D171" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -5959,13 +5951,13 @@
         <v>106</v>
       </c>
       <c r="B172" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="C172" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D172" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5973,13 +5965,13 @@
         <v>106</v>
       </c>
       <c r="B173" t="s">
-        <v>362</v>
+        <v>339</v>
       </c>
       <c r="C173" t="s">
-        <v>111</v>
+        <v>505</v>
       </c>
       <c r="D173" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -5987,13 +5979,13 @@
         <v>106</v>
       </c>
       <c r="B174" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="C174" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D174" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -6001,13 +5993,13 @@
         <v>106</v>
       </c>
       <c r="B175" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C175" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="D175" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -6015,13 +6007,13 @@
         <v>106</v>
       </c>
       <c r="B176" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="C176" t="s">
-        <v>309</v>
+        <v>500</v>
       </c>
       <c r="D176" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -6029,13 +6021,13 @@
         <v>106</v>
       </c>
       <c r="B177" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="C177" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="D177" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -6043,13 +6035,13 @@
         <v>106</v>
       </c>
       <c r="B178" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="C178" t="s">
         <v>107</v>
       </c>
       <c r="D178" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -6057,13 +6049,13 @@
         <v>106</v>
       </c>
       <c r="B179" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="C179" t="s">
-        <v>108</v>
+        <v>504</v>
       </c>
       <c r="D179" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -6071,13 +6063,13 @@
         <v>106</v>
       </c>
       <c r="B180" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C180" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D180" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -6085,13 +6077,13 @@
         <v>106</v>
       </c>
       <c r="B181" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="C181" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D181" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -6099,13 +6091,13 @@
         <v>106</v>
       </c>
       <c r="B182" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="C182" t="s">
-        <v>114</v>
+        <v>486</v>
       </c>
       <c r="D182" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -6113,13 +6105,13 @@
         <v>106</v>
       </c>
       <c r="B183" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="C183" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D183" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -6127,13 +6119,13 @@
         <v>106</v>
       </c>
       <c r="B184" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="C184" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D184" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -6141,13 +6133,13 @@
         <v>106</v>
       </c>
       <c r="B185" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
       <c r="C185" t="s">
-        <v>117</v>
+        <v>488</v>
       </c>
       <c r="D185" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -6155,13 +6147,13 @@
         <v>106</v>
       </c>
       <c r="B186" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="C186" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D186" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -6169,13 +6161,13 @@
         <v>106</v>
       </c>
       <c r="B187" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="C187" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D187" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -6183,13 +6175,13 @@
         <v>106</v>
       </c>
       <c r="B188" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="C188" t="s">
-        <v>120</v>
+        <v>487</v>
       </c>
       <c r="D188" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -6197,13 +6189,13 @@
         <v>106</v>
       </c>
       <c r="B189" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C189" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D189" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -6211,13 +6203,13 @@
         <v>106</v>
       </c>
       <c r="B190" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="C190" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="D190" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -6225,13 +6217,13 @@
         <v>106</v>
       </c>
       <c r="B191" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="C191" t="s">
-        <v>359</v>
+        <v>493</v>
       </c>
       <c r="D191" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -6239,13 +6231,13 @@
         <v>106</v>
       </c>
       <c r="B192" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="C192" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="D192" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -6253,13 +6245,13 @@
         <v>106</v>
       </c>
       <c r="B193" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="C193" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="D193" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -6267,13 +6259,13 @@
         <v>106</v>
       </c>
       <c r="B194" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
       <c r="C194" t="s">
-        <v>303</v>
+        <v>503</v>
       </c>
       <c r="D194" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -6281,13 +6273,13 @@
         <v>106</v>
       </c>
       <c r="B195" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="C195" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="D195" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -6295,13 +6287,13 @@
         <v>106</v>
       </c>
       <c r="B196" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="C196" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D196" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -6309,13 +6301,13 @@
         <v>106</v>
       </c>
       <c r="B197" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="C197" t="s">
-        <v>123</v>
+        <v>492</v>
       </c>
       <c r="D197" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -6323,13 +6315,13 @@
         <v>106</v>
       </c>
       <c r="B198" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="C198" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D198" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -6337,13 +6329,13 @@
         <v>106</v>
       </c>
       <c r="B199" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="C199" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D199" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -6351,13 +6343,13 @@
         <v>106</v>
       </c>
       <c r="B200" t="s">
-        <v>370</v>
+        <v>347</v>
       </c>
       <c r="C200" t="s">
-        <v>126</v>
+        <v>491</v>
       </c>
       <c r="D200" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -6365,13 +6357,13 @@
         <v>106</v>
       </c>
       <c r="B201" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="C201" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D201" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -6379,13 +6371,13 @@
         <v>106</v>
       </c>
       <c r="B202" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="C202" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D202" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -6393,13 +6385,13 @@
         <v>106</v>
       </c>
       <c r="B203" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="C203" t="s">
-        <v>129</v>
+        <v>490</v>
       </c>
       <c r="D203" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -6407,13 +6399,13 @@
         <v>106</v>
       </c>
       <c r="B204" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="C204" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D204" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -6421,13 +6413,13 @@
         <v>106</v>
       </c>
       <c r="B205" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="C205" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="D205" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -6435,13 +6427,13 @@
         <v>106</v>
       </c>
       <c r="B206" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
       <c r="C206" t="s">
-        <v>325</v>
+        <v>489</v>
       </c>
       <c r="D206" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -6449,13 +6441,13 @@
         <v>106</v>
       </c>
       <c r="B207" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C207" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="D207" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -6463,13 +6455,13 @@
         <v>106</v>
       </c>
       <c r="B208" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="C208" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="D208" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -6477,13 +6469,13 @@
         <v>106</v>
       </c>
       <c r="B209" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="C209" t="s">
-        <v>328</v>
+        <v>494</v>
       </c>
       <c r="D209" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -6491,13 +6483,13 @@
         <v>106</v>
       </c>
       <c r="B210" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C210" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="D210" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -6505,13 +6497,13 @@
         <v>106</v>
       </c>
       <c r="B211" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="C211" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D211" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -6519,13 +6511,13 @@
         <v>106</v>
       </c>
       <c r="B212" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
       <c r="C212" t="s">
-        <v>132</v>
+        <v>495</v>
       </c>
       <c r="D212" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -6533,13 +6525,13 @@
         <v>106</v>
       </c>
       <c r="B213" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
       <c r="C213" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D213" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -6547,13 +6539,13 @@
         <v>106</v>
       </c>
       <c r="B214" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="C214" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="D214" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -6561,13 +6553,13 @@
         <v>106</v>
       </c>
       <c r="B215" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="C215" t="s">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="D215" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -6575,13 +6567,13 @@
         <v>106</v>
       </c>
       <c r="B216" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="C216" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="D216" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -6589,13 +6581,13 @@
         <v>106</v>
       </c>
       <c r="B217" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C217" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D217" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -6603,13 +6595,13 @@
         <v>106</v>
       </c>
       <c r="B218" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
       <c r="C218" t="s">
-        <v>135</v>
+        <v>496</v>
       </c>
       <c r="D218" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -6617,13 +6609,13 @@
         <v>106</v>
       </c>
       <c r="B219" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="C219" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D219" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -6631,13 +6623,13 @@
         <v>106</v>
       </c>
       <c r="B220" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="C220" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D220" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -6645,13 +6637,13 @@
         <v>106</v>
       </c>
       <c r="B221" t="s">
-        <v>369</v>
+        <v>346</v>
       </c>
       <c r="C221" t="s">
-        <v>138</v>
+        <v>502</v>
       </c>
       <c r="D221" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -6659,13 +6651,13 @@
         <v>106</v>
       </c>
       <c r="B222" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="C222" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D222" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -6673,13 +6665,13 @@
         <v>106</v>
       </c>
       <c r="B223" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="C223" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D223" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -6687,13 +6679,13 @@
         <v>106</v>
       </c>
       <c r="B224" t="s">
-        <v>368</v>
+        <v>345</v>
       </c>
       <c r="C224" t="s">
-        <v>141</v>
+        <v>501</v>
       </c>
       <c r="D224" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -6701,13 +6693,13 @@
         <v>106</v>
       </c>
       <c r="B225" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="C225" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D225" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -6715,13 +6707,13 @@
         <v>106</v>
       </c>
       <c r="B226" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="C226" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="D226" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -6729,13 +6721,13 @@
         <v>106</v>
       </c>
       <c r="B227" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="C227" t="s">
-        <v>346</v>
+        <v>499</v>
       </c>
       <c r="D227" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -6743,13 +6735,13 @@
         <v>106</v>
       </c>
       <c r="B228" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
       <c r="C228" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="D228" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -6757,13 +6749,13 @@
         <v>106</v>
       </c>
       <c r="B229" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="C229" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="D229" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -6771,13 +6763,13 @@
         <v>106</v>
       </c>
       <c r="B230" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
       <c r="C230" t="s">
-        <v>336</v>
+        <v>498</v>
       </c>
       <c r="D230" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -6785,13 +6777,13 @@
         <v>106</v>
       </c>
       <c r="B231" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="C231" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
       <c r="D231" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -6799,13 +6791,13 @@
         <v>106</v>
       </c>
       <c r="B232" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="C232" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D232" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -6813,13 +6805,13 @@
         <v>106</v>
       </c>
       <c r="B233" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="C233" t="s">
-        <v>144</v>
+        <v>497</v>
       </c>
       <c r="D233" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -6827,13 +6819,13 @@
         <v>106</v>
       </c>
       <c r="B234" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="C234" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D234" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -6841,13 +6833,13 @@
         <v>2</v>
       </c>
       <c r="B235" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
       <c r="C235" t="s">
         <v>0</v>
       </c>
       <c r="D235" t="s">
-        <v>484</v>
+        <v>461</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -6855,13 +6847,13 @@
         <v>2</v>
       </c>
       <c r="B236" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="C236" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="D236" t="s">
-        <v>484</v>
+        <v>461</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -6869,13 +6861,13 @@
         <v>2</v>
       </c>
       <c r="B237" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="C237" t="s">
         <v>1</v>
       </c>
       <c r="D237" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -6883,13 +6875,13 @@
         <v>83</v>
       </c>
       <c r="B238" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="C238" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="D238" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -6897,13 +6889,13 @@
         <v>83</v>
       </c>
       <c r="B239" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="C239" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="D239" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -6911,13 +6903,13 @@
         <v>83</v>
       </c>
       <c r="B240" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="C240" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="D240" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -6925,13 +6917,13 @@
         <v>83</v>
       </c>
       <c r="B241" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
       <c r="C241" t="s">
         <v>84</v>
       </c>
       <c r="D241" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -6939,13 +6931,13 @@
         <v>69</v>
       </c>
       <c r="B242" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="C242" t="s">
         <v>70</v>
       </c>
       <c r="D242" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -6953,13 +6945,13 @@
         <v>69</v>
       </c>
       <c r="B243" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="C243" t="s">
         <v>71</v>
       </c>
       <c r="D243" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -6967,13 +6959,13 @@
         <v>69</v>
       </c>
       <c r="B244" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
       <c r="C244" t="s">
         <v>72</v>
       </c>
       <c r="D244" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -6981,13 +6973,13 @@
         <v>69</v>
       </c>
       <c r="B245" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="C245" t="s">
         <v>73</v>
       </c>
       <c r="D245" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -6995,13 +6987,13 @@
         <v>69</v>
       </c>
       <c r="B246" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="C246" t="s">
         <v>74</v>
       </c>
       <c r="D246" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -7009,13 +7001,13 @@
         <v>69</v>
       </c>
       <c r="B247" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="C247" t="s">
         <v>75</v>
       </c>
       <c r="D247" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -7023,13 +7015,13 @@
         <v>69</v>
       </c>
       <c r="B248" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="C248" t="s">
         <v>76</v>
       </c>
       <c r="D248" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -7037,13 +7029,13 @@
         <v>69</v>
       </c>
       <c r="B249" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="C249" t="s">
         <v>77</v>
       </c>
       <c r="D249" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -7058,7 +7050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2788C3-640F-43AF-AA5B-63ED02B26D58}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -7070,17 +7062,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="4">
+        <v>135</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
     </row>
@@ -7088,7 +7080,7 @@
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>9</v>
       </c>
     </row>
@@ -7096,7 +7088,7 @@
       <c r="A4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>50</v>
       </c>
     </row>
@@ -7104,7 +7096,7 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>64</v>
       </c>
     </row>
@@ -7112,15 +7104,15 @@
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" s="4">
+        <v>137</v>
+      </c>
+      <c r="B7">
         <v>37</v>
       </c>
     </row>
@@ -7128,7 +7120,7 @@
       <c r="A8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>67</v>
       </c>
     </row>
@@ -7136,7 +7128,7 @@
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>3</v>
       </c>
     </row>
@@ -7144,7 +7136,7 @@
       <c r="A10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>4</v>
       </c>
     </row>
@@ -7152,7 +7144,7 @@
       <c r="A11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>8</v>
       </c>
     </row>
@@ -7160,7 +7152,7 @@
       <c r="A12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>248</v>
       </c>
     </row>

</xml_diff>